<commit_message>
Update Evaluation Metrics And Results
</commit_message>
<xml_diff>
--- a/eval/results/results.xlsx
+++ b/eval/results/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Java\link-shortener\eval\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5492EE-96F6-40F9-B202-A1A6B35F7816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF569FED-6374-45F1-AAD2-107E9EC0CB14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{1F731DB4-3E6E-49F6-8898-DBE4A72A56EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{1F731DB4-3E6E-49F6-8898-DBE4A72A56EE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TEST 1" sheetId="1" r:id="rId1"/>
+    <sheet name="TEST 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>Tool</t>
   </si>
@@ -66,40 +67,37 @@
     <t>1/1s</t>
   </si>
   <si>
-    <t>TEST 1</t>
-  </si>
-  <si>
-    <t>Create Only</t>
-  </si>
-  <si>
     <t>With Rate Limiting</t>
   </si>
   <si>
     <t>Without Rate Limiting</t>
   </si>
   <si>
-    <t>LATENCY</t>
-  </si>
-  <si>
     <t>RPS</t>
   </si>
   <si>
-    <t>CPU USAGE</t>
-  </si>
-  <si>
-    <t>RAM USAGE</t>
-  </si>
-  <si>
-    <t>TEST 2</t>
-  </si>
-  <si>
-    <t>TEST 3</t>
-  </si>
-  <si>
-    <t>Random 50/50</t>
-  </si>
-  <si>
-    <t>Get Only</t>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>100ms</t>
+  </si>
+  <si>
+    <t>LATENCY (ms)</t>
+  </si>
+  <si>
+    <t>CPU USAGE (%)</t>
+  </si>
+  <si>
+    <t>RAM USAGE (MB)</t>
+  </si>
+  <si>
+    <t>CREATE ONLY</t>
+  </si>
+  <si>
+    <t>GET ONLY</t>
+  </si>
+  <si>
+    <t>50/50</t>
   </si>
 </sst>
 </file>
@@ -488,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A48D05C-7533-476F-8E73-14CB279FF17A}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,38 +529,42 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>10</v>
-      </c>
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -571,32 +573,24 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3">
-        <v>5.78</v>
-      </c>
-      <c r="C12" s="3">
-        <v>51.19</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -604,42 +598,48 @@
         <v>15</v>
       </c>
       <c r="B13" s="3">
-        <v>8425.16</v>
+        <v>4.74</v>
       </c>
       <c r="C13" s="3">
-        <v>972.81</v>
+        <v>11.43</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>512.04999999999995</v>
+        <v>475.02</v>
       </c>
       <c r="C14" s="3">
-        <v>228.18</v>
+        <v>446.69</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>107.2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>160.97999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
-        <v>1102.8</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1196.97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3">
+        <v>907.95</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1162.52</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
@@ -647,32 +647,24 @@
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="C21" s="3">
-        <v>4.95</v>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -680,38 +672,44 @@
         <v>15</v>
       </c>
       <c r="B22" s="3">
-        <v>6818.65</v>
+        <v>3.8</v>
       </c>
       <c r="C22" s="3">
-        <v>9878.6200000000008</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B23" s="3">
-        <v>727.23</v>
+        <v>479.52</v>
       </c>
       <c r="C23" s="3">
-        <v>837.79</v>
+        <v>475.77</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3">
+        <v>132.81</v>
+      </c>
+      <c r="C24" s="3">
+        <v>162.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="3">
-        <v>1649.44</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1722.08</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="B25" s="3">
+        <v>1033.6199999999999</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1323.04</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
@@ -724,32 +722,24 @@
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3">
-        <v>5.6</v>
-      </c>
-      <c r="C30" s="3">
-        <v>23.6</v>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -757,36 +747,354 @@
         <v>15</v>
       </c>
       <c r="B31" s="3">
-        <v>8704.9599999999991</v>
+        <v>3.39</v>
       </c>
       <c r="C31" s="3">
-        <v>2104.65</v>
+        <v>7.47</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B32" s="3">
-        <v>543.70000000000005</v>
+        <v>481.35</v>
       </c>
       <c r="C32" s="3">
-        <v>252.87</v>
+        <v>463.18</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="3">
+        <v>61.89</v>
+      </c>
+      <c r="C33" s="3">
+        <v>85.12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="3">
-        <v>1766.43</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1869.7</v>
+      <c r="B34" s="3">
+        <v>1048.81</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1350.93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38DA6BD-D998-48F3-B000-21ED2D24F898}">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="32.6328125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>500</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="C13" s="3">
+        <v>307.83999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4611.43</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1214.97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>255.2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>192.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1175.3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1485.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3">
+        <v>9.65</v>
+      </c>
+      <c r="C22" s="3">
+        <v>113.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4525.91</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2322.62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3">
+        <v>412.1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>484.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1681.31</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1913.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="3">
+        <v>4.12</v>
+      </c>
+      <c r="C31" s="3">
+        <v>247.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3">
+        <v>4762.03</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1428.14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="3">
+        <v>212.03</v>
+      </c>
+      <c r="C33" s="3">
+        <v>233.45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1789.37</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2005.82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>